<commit_message>
Removing totals in tags of measures in example files. Updating version and changelog.
</commit_message>
<xml_diff>
--- a/doc/_static/example-files/PMHC-4-0-combined.xlsx
+++ b/doc/_static/example-files/PMHC-4-0-combined.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="349">
   <si>
     <t>key</t>
   </si>
@@ -287,42 +287,27 @@
     <t>3+</t>
   </si>
   <si>
-    <t>total=3+</t>
-  </si>
-  <si>
     <t>IarDstIM01</t>
   </si>
   <si>
     <t>IarDstIM02</t>
   </si>
   <si>
-    <t>total=2</t>
-  </si>
-  <si>
     <t>IarDstIM03</t>
   </si>
   <si>
     <t>2+</t>
   </si>
   <si>
-    <t>total=2+</t>
-  </si>
-  <si>
     <t>IarDstIM04</t>
   </si>
   <si>
-    <t>total=5</t>
-  </si>
-  <si>
     <t>IarDstIM05</t>
   </si>
   <si>
     <t>IarDstIM06</t>
   </si>
   <si>
-    <t>total=1</t>
-  </si>
-  <si>
     <t>IarDstIM07</t>
   </si>
   <si>
@@ -332,9 +317,6 @@
     <t>4+</t>
   </si>
   <si>
-    <t>total=4+</t>
-  </si>
-  <si>
     <t>IarDstIM09</t>
   </si>
   <si>
@@ -599,33 +581,18 @@
     <t>K10M400</t>
   </si>
   <si>
-    <t>total=25</t>
-  </si>
-  <si>
     <t>K10M401</t>
   </si>
   <si>
-    <t>total=30</t>
-  </si>
-  <si>
     <t>K10M402</t>
   </si>
   <si>
-    <t>total=39</t>
-  </si>
-  <si>
     <t>K10M403</t>
   </si>
   <si>
-    <t>total=31</t>
-  </si>
-  <si>
     <t>K10M404</t>
   </si>
   <si>
-    <t>total=29</t>
-  </si>
-  <si>
     <t>k5_item1</t>
   </si>
   <si>
@@ -650,15 +617,9 @@
     <t>K5M400</t>
   </si>
   <si>
-    <t>total=99</t>
-  </si>
-  <si>
     <t>K5M401</t>
   </si>
   <si>
-    <t>total=14</t>
-  </si>
-  <si>
     <t>K5M402</t>
   </si>
   <si>
@@ -671,15 +632,9 @@
     <t>K5M405</t>
   </si>
   <si>
-    <t>total=12</t>
-  </si>
-  <si>
     <t>K5M406</t>
   </si>
   <si>
-    <t>total=16</t>
-  </si>
-  <si>
     <t>K5M407</t>
   </si>
   <si>
@@ -848,33 +803,21 @@
     <t>PY101</t>
   </si>
   <si>
-    <t>total=18</t>
-  </si>
-  <si>
     <t>SDQM401</t>
   </si>
   <si>
     <t>PC201</t>
   </si>
   <si>
-    <t>total=13</t>
-  </si>
-  <si>
     <t>SDQM402</t>
   </si>
   <si>
-    <t>total=22</t>
-  </si>
-  <si>
     <t>SDQM403</t>
   </si>
   <si>
     <t>PC101</t>
   </si>
   <si>
-    <t>total=17</t>
-  </si>
-  <si>
     <t>SDQM404</t>
   </si>
   <si>
@@ -884,27 +827,15 @@
     <t>SDQM405</t>
   </si>
   <si>
-    <t>total=20</t>
-  </si>
-  <si>
     <t>SDQM406</t>
   </si>
   <si>
-    <t>total=19</t>
-  </si>
-  <si>
     <t>SDQM407</t>
   </si>
   <si>
-    <t>total=15</t>
-  </si>
-  <si>
     <t>SDQM408</t>
   </si>
   <si>
-    <t>total=26</t>
-  </si>
-  <si>
     <t>SDQM409</t>
   </si>
   <si>
@@ -920,9 +851,6 @@
     <t>SDQM413</t>
   </si>
   <si>
-    <t>total=21</t>
-  </si>
-  <si>
     <t>SDQM414</t>
   </si>
   <si>
@@ -933,9 +861,6 @@
   </si>
   <si>
     <t>SDQM416</t>
-  </si>
-  <si>
-    <t>total=27</t>
   </si>
   <si>
     <t>SDQM417</t>
@@ -1531,28 +1456,28 @@
         <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="E1" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="F1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G1" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="H1" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="I1" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="J1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1560,10 +1485,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -1583,19 +1508,16 @@
       <c r="I2">
         <v>99</v>
       </c>
-      <c r="J2" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1615,19 +1537,16 @@
       <c r="I3">
         <v>14</v>
       </c>
-      <c r="J3" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D4">
         <v>9</v>
@@ -1647,19 +1566,16 @@
       <c r="I4">
         <v>99</v>
       </c>
-      <c r="J4" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1679,19 +1595,16 @@
       <c r="I5">
         <v>99</v>
       </c>
-      <c r="J5" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1711,19 +1624,16 @@
       <c r="I6">
         <v>99</v>
       </c>
-      <c r="J6" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -1743,19 +1653,16 @@
       <c r="I7">
         <v>12</v>
       </c>
-      <c r="J7" t="s">
-        <v>214</v>
-      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1775,19 +1682,16 @@
       <c r="I8">
         <v>16</v>
       </c>
-      <c r="J8" t="s">
-        <v>216</v>
-      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="C9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1807,19 +1711,16 @@
       <c r="I9">
         <v>99</v>
       </c>
-      <c r="J9" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1839,19 +1740,16 @@
       <c r="I10">
         <v>12</v>
       </c>
-      <c r="J10" t="s">
-        <v>214</v>
-      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1870,9 +1768,6 @@
       </c>
       <c r="I11">
         <v>99</v>
-      </c>
-      <c r="J11" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -1896,160 +1791,160 @@
         <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J1" t="s">
+        <v>211</v>
+      </c>
+      <c r="K1" t="s">
+        <v>212</v>
+      </c>
+      <c r="L1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N1" t="s">
+        <v>215</v>
+      </c>
+      <c r="O1" t="s">
+        <v>216</v>
+      </c>
+      <c r="P1" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>218</v>
+      </c>
+      <c r="R1" t="s">
+        <v>219</v>
+      </c>
+      <c r="S1" t="s">
         <v>220</v>
       </c>
-      <c r="E1" t="s">
+      <c r="T1" t="s">
         <v>221</v>
       </c>
-      <c r="F1" t="s">
+      <c r="U1" t="s">
         <v>222</v>
       </c>
-      <c r="G1" t="s">
+      <c r="V1" t="s">
         <v>223</v>
       </c>
-      <c r="H1" t="s">
+      <c r="W1" t="s">
         <v>224</v>
       </c>
-      <c r="I1" t="s">
+      <c r="X1" t="s">
         <v>225</v>
       </c>
-      <c r="J1" t="s">
+      <c r="Y1" t="s">
         <v>226</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Z1" t="s">
         <v>227</v>
       </c>
-      <c r="L1" t="s">
+      <c r="AA1" t="s">
         <v>228</v>
       </c>
-      <c r="M1" t="s">
+      <c r="AB1" t="s">
         <v>229</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AC1" t="s">
         <v>230</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AD1" t="s">
         <v>231</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AE1" t="s">
         <v>232</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AF1" t="s">
         <v>233</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AG1" t="s">
         <v>234</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AH1" t="s">
         <v>235</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AI1" t="s">
         <v>236</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AJ1" t="s">
         <v>237</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AK1" t="s">
         <v>238</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AL1" t="s">
         <v>239</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AM1" t="s">
         <v>240</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AN1" t="s">
         <v>241</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AO1" t="s">
         <v>242</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AP1" t="s">
         <v>243</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AQ1" t="s">
         <v>244</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AR1" t="s">
         <v>245</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AS1" t="s">
         <v>246</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AT1" t="s">
         <v>247</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AU1" t="s">
         <v>248</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AV1" t="s">
         <v>249</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AW1" t="s">
         <v>250</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AX1" t="s">
         <v>251</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AY1" t="s">
         <v>252</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AZ1" t="s">
         <v>253</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BA1" t="s">
         <v>254</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="BB1" t="s">
         <v>255</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>256</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>257</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>258</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>259</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>260</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>261</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>262</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>263</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>264</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>265</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>266</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>267</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>268</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>269</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:54">
@@ -2057,13 +1952,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D2" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2212,22 +2107,19 @@
       <c r="BA2">
         <v>8</v>
       </c>
-      <c r="BB2" t="s">
-        <v>273</v>
-      </c>
     </row>
     <row r="3" spans="1:54">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D3" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2376,22 +2268,19 @@
       <c r="BA3">
         <v>7</v>
       </c>
-      <c r="BB3" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="4" spans="1:54">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D4" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2540,22 +2429,19 @@
       <c r="BA4">
         <v>4</v>
       </c>
-      <c r="BB4" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="5" spans="1:54">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="C5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D5" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2704,22 +2590,19 @@
       <c r="BA5">
         <v>3</v>
       </c>
-      <c r="BB5" t="s">
-        <v>281</v>
-      </c>
     </row>
     <row r="6" spans="1:54">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D6" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2868,22 +2751,19 @@
       <c r="BA6">
         <v>1</v>
       </c>
-      <c r="BB6" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="7" spans="1:54">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D7" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3032,22 +2912,19 @@
       <c r="BA7">
         <v>5</v>
       </c>
-      <c r="BB7" t="s">
-        <v>285</v>
-      </c>
     </row>
     <row r="8" spans="1:54">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3196,22 +3073,19 @@
       <c r="BA8">
         <v>2</v>
       </c>
-      <c r="BB8" t="s">
-        <v>287</v>
-      </c>
     </row>
     <row r="9" spans="1:54">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D9" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -3360,22 +3234,19 @@
       <c r="BA9">
         <v>0</v>
       </c>
-      <c r="BB9" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="10" spans="1:54">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="C10" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D10" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -3524,22 +3395,19 @@
       <c r="BA10">
         <v>0</v>
       </c>
-      <c r="BB10" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="11" spans="1:54">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>283</v>
+        <v>264</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -3688,22 +3556,19 @@
       <c r="BA11">
         <v>5</v>
       </c>
-      <c r="BB11" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="12" spans="1:54">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3852,22 +3717,19 @@
       <c r="BA12">
         <v>0</v>
       </c>
-      <c r="BB12" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="13" spans="1:54">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -4016,22 +3878,19 @@
       <c r="BA13">
         <v>0</v>
       </c>
-      <c r="BB13" t="s">
-        <v>281</v>
-      </c>
     </row>
     <row r="14" spans="1:54">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="C14" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D14" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -4180,22 +4039,19 @@
       <c r="BA14">
         <v>4</v>
       </c>
-      <c r="BB14" t="s">
-        <v>281</v>
-      </c>
     </row>
     <row r="15" spans="1:54">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>296</v>
+        <v>273</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D15" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -4344,22 +4200,19 @@
       <c r="BA15">
         <v>4</v>
       </c>
-      <c r="BB15" t="s">
-        <v>297</v>
-      </c>
     </row>
     <row r="16" spans="1:54">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="C16" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D16" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -4508,22 +4361,19 @@
       <c r="BA16">
         <v>3</v>
       </c>
-      <c r="BB16" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="17" spans="1:54">
+    </row>
+    <row r="17" spans="1:53">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="C17" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D17" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -4672,22 +4522,19 @@
       <c r="BA17">
         <v>4</v>
       </c>
-      <c r="BB17" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="18" spans="1:54">
+    </row>
+    <row r="18" spans="1:53">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="C18" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D18" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -4836,22 +4683,19 @@
       <c r="BA18">
         <v>4</v>
       </c>
-      <c r="BB18" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="19" spans="1:54">
+    </row>
+    <row r="19" spans="1:53">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D19" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -5000,22 +4844,19 @@
       <c r="BA19">
         <v>0</v>
       </c>
-      <c r="BB19" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="20" spans="1:54">
+    </row>
+    <row r="20" spans="1:53">
       <c r="A20" t="s">
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
       <c r="C20" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D20" t="s">
-        <v>305</v>
+        <v>280</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -5164,22 +5005,19 @@
       <c r="BA20">
         <v>2</v>
       </c>
-      <c r="BB20" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="21" spans="1:54">
+    </row>
+    <row r="21" spans="1:53">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D21" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -5328,22 +5166,19 @@
       <c r="BA21">
         <v>0</v>
       </c>
-      <c r="BB21" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="22" spans="1:54">
+    </row>
+    <row r="22" spans="1:53">
       <c r="A22" t="s">
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="C22" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D22" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -5491,9 +5326,6 @@
       </c>
       <c r="BA22">
         <v>2</v>
-      </c>
-      <c r="BB22" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -5514,55 +5346,55 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>308</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>309</v>
+        <v>284</v>
       </c>
       <c r="E1" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
       <c r="F1" t="s">
-        <v>311</v>
+        <v>286</v>
       </c>
       <c r="G1" t="s">
-        <v>312</v>
+        <v>287</v>
       </c>
       <c r="H1" t="s">
-        <v>313</v>
+        <v>288</v>
       </c>
       <c r="I1" t="s">
-        <v>314</v>
+        <v>289</v>
       </c>
       <c r="J1" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
       <c r="K1" t="s">
-        <v>316</v>
+        <v>291</v>
       </c>
       <c r="L1" t="s">
-        <v>317</v>
+        <v>292</v>
       </c>
       <c r="M1" t="s">
-        <v>318</v>
+        <v>293</v>
       </c>
       <c r="N1" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="O1" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
       <c r="P1" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
       <c r="Q1" t="s">
-        <v>322</v>
+        <v>297</v>
       </c>
       <c r="R1" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -5570,10 +5402,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D2">
         <v>17052021</v>
@@ -5612,7 +5444,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>325</v>
+        <v>300</v>
       </c>
       <c r="Q2">
         <v>400</v>
@@ -5623,10 +5455,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D3">
         <v>17122021</v>
@@ -5665,7 +5497,7 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>327</v>
+        <v>302</v>
       </c>
       <c r="Q3">
         <v>100</v>
@@ -5676,10 +5508,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
+        <v>303</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D4">
         <v>28032021</v>
@@ -5718,7 +5550,7 @@
         <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>329</v>
+        <v>304</v>
       </c>
       <c r="Q4">
         <v>200</v>
@@ -5729,10 +5561,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>330</v>
+        <v>305</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D5">
         <v>17052021</v>
@@ -5771,7 +5603,7 @@
         <v>2</v>
       </c>
       <c r="P5" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
       <c r="Q5">
         <v>100</v>
@@ -5782,10 +5614,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>332</v>
+        <v>307</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D6">
         <v>3082021</v>
@@ -5824,7 +5656,7 @@
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
       <c r="Q6">
         <v>400</v>
@@ -5835,10 +5667,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>334</v>
+        <v>309</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D7">
         <v>17112021</v>
@@ -5877,7 +5709,7 @@
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>335</v>
+        <v>310</v>
       </c>
       <c r="Q7">
         <v>100</v>
@@ -5888,10 +5720,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>336</v>
+        <v>311</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D8">
         <v>12082021</v>
@@ -5930,7 +5762,7 @@
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
       <c r="Q8">
         <v>100</v>
@@ -5941,10 +5773,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>337</v>
+        <v>312</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D9">
         <v>11012022</v>
@@ -5983,7 +5815,7 @@
         <v>2</v>
       </c>
       <c r="P9" t="s">
-        <v>338</v>
+        <v>313</v>
       </c>
       <c r="Q9">
         <v>300</v>
@@ -5994,10 +5826,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>339</v>
+        <v>314</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D10">
         <v>28062021</v>
@@ -6036,7 +5868,7 @@
         <v>2</v>
       </c>
       <c r="P10" t="s">
-        <v>340</v>
+        <v>315</v>
       </c>
       <c r="Q10">
         <v>200</v>
@@ -6047,10 +5879,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>341</v>
+        <v>316</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D11">
         <v>17082021</v>
@@ -6089,7 +5921,7 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>340</v>
+        <v>315</v>
       </c>
       <c r="Q11">
         <v>200</v>
@@ -6113,16 +5945,16 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>342</v>
+        <v>317</v>
       </c>
       <c r="C1" t="s">
-        <v>308</v>
+        <v>283</v>
       </c>
       <c r="D1" t="s">
-        <v>343</v>
+        <v>318</v>
       </c>
       <c r="E1" t="s">
-        <v>344</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -6130,13 +5962,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>345</v>
+        <v>320</v>
       </c>
       <c r="C2" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="D2" t="s">
-        <v>346</v>
+        <v>321</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -6147,13 +5979,13 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>347</v>
+        <v>322</v>
       </c>
       <c r="C3" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
       <c r="D3" t="s">
-        <v>348</v>
+        <v>323</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6164,13 +5996,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>349</v>
+        <v>324</v>
       </c>
       <c r="C4" t="s">
-        <v>328</v>
+        <v>303</v>
       </c>
       <c r="D4" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6181,13 +6013,13 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>351</v>
+        <v>326</v>
       </c>
       <c r="C5" t="s">
-        <v>330</v>
+        <v>305</v>
       </c>
       <c r="D5" t="s">
-        <v>352</v>
+        <v>327</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6198,13 +6030,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>353</v>
+        <v>328</v>
       </c>
       <c r="C6" t="s">
-        <v>332</v>
+        <v>307</v>
       </c>
       <c r="D6" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6215,13 +6047,13 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>355</v>
+        <v>330</v>
       </c>
       <c r="C7" t="s">
-        <v>334</v>
+        <v>309</v>
       </c>
       <c r="D7" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6232,13 +6064,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>357</v>
+        <v>332</v>
       </c>
       <c r="C8" t="s">
-        <v>336</v>
+        <v>311</v>
       </c>
       <c r="D8" t="s">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -6249,13 +6081,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>359</v>
+        <v>334</v>
       </c>
       <c r="C9" t="s">
-        <v>337</v>
+        <v>312</v>
       </c>
       <c r="D9" t="s">
-        <v>360</v>
+        <v>335</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -6266,13 +6098,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>361</v>
+        <v>336</v>
       </c>
       <c r="C10" t="s">
-        <v>339</v>
+        <v>314</v>
       </c>
       <c r="D10" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6283,13 +6115,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>363</v>
+        <v>338</v>
       </c>
       <c r="C11" t="s">
-        <v>341</v>
+        <v>316</v>
       </c>
       <c r="D11" t="s">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -6300,13 +6132,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="C12" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
       <c r="D12" t="s">
-        <v>348</v>
+        <v>323</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -6317,13 +6149,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>366</v>
+        <v>341</v>
       </c>
       <c r="C13" t="s">
-        <v>341</v>
+        <v>316</v>
       </c>
       <c r="D13" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -6347,28 +6179,28 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1" t="s">
         <v>343</v>
       </c>
-      <c r="C1" t="s">
-        <v>367</v>
-      </c>
-      <c r="D1" t="s">
-        <v>368</v>
-      </c>
       <c r="E1" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="F1" t="s">
-        <v>370</v>
+        <v>345</v>
       </c>
       <c r="G1" t="s">
-        <v>371</v>
+        <v>346</v>
       </c>
       <c r="H1" t="s">
-        <v>372</v>
+        <v>347</v>
       </c>
       <c r="I1" t="s">
-        <v>373</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6376,7 +6208,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>346</v>
+        <v>321</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -6402,7 +6234,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>348</v>
+        <v>323</v>
       </c>
       <c r="C3">
         <v>99</v>
@@ -6428,7 +6260,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -6454,7 +6286,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>352</v>
+        <v>327</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -6480,7 +6312,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -6506,7 +6338,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>356</v>
+        <v>331</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -6532,7 +6364,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>358</v>
+        <v>333</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -6558,7 +6390,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>360</v>
+        <v>335</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6584,7 +6416,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="C10">
         <v>11</v>
@@ -6610,7 +6442,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -7483,16 +7315,13 @@
       <c r="N2">
         <v>3</v>
       </c>
-      <c r="O2" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>53</v>
@@ -7530,16 +7359,13 @@
       <c r="N3">
         <v>9</v>
       </c>
-      <c r="O3" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>55</v>
@@ -7577,16 +7403,13 @@
       <c r="N4">
         <v>2</v>
       </c>
-      <c r="O4" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>57</v>
@@ -7619,13 +7442,10 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N5">
         <v>3</v>
-      </c>
-      <c r="O5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -7633,7 +7453,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
         <v>59</v>
@@ -7671,16 +7491,13 @@
       <c r="N6">
         <v>5</v>
       </c>
-      <c r="O6" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C7" t="s">
         <v>61</v>
@@ -7713,13 +7530,10 @@
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N7">
         <v>3</v>
-      </c>
-      <c r="O7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -7727,7 +7541,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
         <v>63</v>
@@ -7765,16 +7579,13 @@
       <c r="N8">
         <v>9</v>
       </c>
-      <c r="O8" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
         <v>65</v>
@@ -7812,16 +7623,13 @@
       <c r="N9">
         <v>1</v>
       </c>
-      <c r="O9" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
         <v>67</v>
@@ -7854,21 +7662,18 @@
         <v>4</v>
       </c>
       <c r="M10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N10">
         <v>4</v>
       </c>
-      <c r="O10" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
         <v>69</v>
@@ -7905,9 +7710,6 @@
       </c>
       <c r="N11">
         <v>3</v>
-      </c>
-      <c r="O11" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -7928,19 +7730,19 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
         <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s">
         <v>40</v>
@@ -7949,58 +7751,58 @@
         <v>41</v>
       </c>
       <c r="I1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" t="s">
         <v>106</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>107</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>108</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>109</v>
-      </c>
-      <c r="M1" t="s">
-        <v>110</v>
-      </c>
-      <c r="N1" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" t="s">
-        <v>112</v>
-      </c>
-      <c r="P1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>114</v>
-      </c>
-      <c r="R1" t="s">
-        <v>115</v>
       </c>
       <c r="S1" t="s">
         <v>46</v>
       </c>
       <c r="T1" t="s">
+        <v>110</v>
+      </c>
+      <c r="U1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V1" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" t="s">
+        <v>113</v>
+      </c>
+      <c r="X1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z1" t="s">
         <v>116</v>
-      </c>
-      <c r="U1" t="s">
-        <v>117</v>
-      </c>
-      <c r="V1" t="s">
-        <v>118</v>
-      </c>
-      <c r="W1" t="s">
-        <v>119</v>
-      </c>
-      <c r="X1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>122</v>
       </c>
       <c r="AA1" t="s">
         <v>42</v>
@@ -8009,10 +7811,10 @@
         <v>43</v>
       </c>
       <c r="AC1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="AD1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -8020,7 +7822,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -8101,7 +7903,7 @@
         <v>7</v>
       </c>
       <c r="AC2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -8109,7 +7911,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -8190,10 +7992,10 @@
         <v>4</v>
       </c>
       <c r="AC3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="AD3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -8201,7 +8003,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
@@ -8282,7 +8084,7 @@
         <v>4</v>
       </c>
       <c r="AC4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -8290,7 +8092,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -8371,7 +8173,7 @@
         <v>6</v>
       </c>
       <c r="AC5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -8379,7 +8181,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
         <v>32</v>
@@ -8460,7 +8262,7 @@
         <v>8</v>
       </c>
       <c r="AC6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -8468,7 +8270,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -8546,7 +8348,7 @@
         <v>8</v>
       </c>
       <c r="AC7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -8554,7 +8356,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
@@ -8635,7 +8437,7 @@
         <v>5</v>
       </c>
       <c r="AC8" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -8643,7 +8445,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
@@ -8724,7 +8526,7 @@
         <v>9</v>
       </c>
       <c r="AC9" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -8732,7 +8534,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
         <v>36</v>
@@ -8813,7 +8615,7 @@
         <v>5</v>
       </c>
       <c r="AC10" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -8821,7 +8623,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
@@ -8899,7 +8701,7 @@
         <v>8</v>
       </c>
       <c r="AC11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -8917,13 +8719,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
         <v>38</v>
@@ -8934,7 +8736,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -8948,7 +8750,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -8962,7 +8764,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -8976,7 +8778,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -8990,7 +8792,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -9004,7 +8806,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -9018,7 +8820,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -9032,7 +8834,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -9046,7 +8848,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -9060,7 +8862,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -9087,19 +8889,19 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -9107,10 +8909,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D2">
         <v>27012021</v>
@@ -9124,10 +8926,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D3">
         <v>6022021</v>
@@ -9141,10 +8943,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D4">
         <v>26092020</v>
@@ -9158,10 +8960,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D5">
         <v>19012021</v>
@@ -9175,10 +8977,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D6">
         <v>17032021</v>
@@ -9192,10 +8994,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D7">
         <v>20102020</v>
@@ -9209,10 +9011,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D8">
         <v>4062021</v>
@@ -9226,10 +9028,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D9">
         <v>16082020</v>
@@ -9243,10 +9045,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D10">
         <v>1072021</v>
@@ -9260,10 +9062,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D11">
         <v>26092020</v>
@@ -9277,10 +9079,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D12">
         <v>6082020</v>
@@ -9294,10 +9096,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D13">
         <v>21032021</v>
@@ -9311,10 +9113,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D14">
         <v>18012021</v>
@@ -9328,10 +9130,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D15">
         <v>21012021</v>
@@ -9345,10 +9147,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D16">
         <v>17082020</v>
@@ -9362,10 +9164,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D17">
         <v>15122020</v>
@@ -9379,10 +9181,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D18">
         <v>22102020</v>
@@ -9396,10 +9198,10 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D19">
         <v>25102020</v>
@@ -9413,10 +9215,10 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D20">
         <v>26042021</v>
@@ -9430,10 +9232,10 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C21" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D21">
         <v>19082020</v>
@@ -9447,10 +9249,10 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D22">
         <v>27072021</v>
@@ -9480,55 +9282,55 @@
         <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" t="s">
         <v>173</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>174</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>175</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>176</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>177</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>178</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>179</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>180</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>181</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>182</v>
-      </c>
-      <c r="N1" t="s">
-        <v>183</v>
-      </c>
-      <c r="O1" t="s">
-        <v>184</v>
-      </c>
-      <c r="P1" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>186</v>
-      </c>
-      <c r="R1" t="s">
-        <v>187</v>
-      </c>
-      <c r="S1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -9536,10 +9338,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -9586,19 +9388,16 @@
       <c r="R2">
         <v>25</v>
       </c>
-      <c r="S2" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -9645,19 +9444,16 @@
       <c r="R3">
         <v>30</v>
       </c>
-      <c r="S3" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -9704,19 +9500,16 @@
       <c r="R4">
         <v>39</v>
       </c>
-      <c r="S4" t="s">
-        <v>194</v>
-      </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -9763,19 +9556,16 @@
       <c r="R5">
         <v>31</v>
       </c>
-      <c r="S5" t="s">
-        <v>196</v>
-      </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -9821,9 +9611,6 @@
       </c>
       <c r="R6">
         <v>29</v>
-      </c>
-      <c r="S6" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* Added Changes and Upgrading from Version 2 * Removed Funding Source from Intake example files
</commit_message>
<xml_diff>
--- a/doc/_static/example-files/PMHC-4-0-combined.xlsx
+++ b/doc/_static/example-files/PMHC-4-0-combined.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="348">
   <si>
     <t>key</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>date_client_contacted_intake</t>
-  </si>
-  <si>
-    <t>intake_funding_source</t>
   </si>
   <si>
     <t>suicide_referral_flag</t>
@@ -1453,31 +1450,31 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" t="s">
         <v>188</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>189</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>190</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>191</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>192</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>193</v>
-      </c>
-      <c r="J1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1485,10 +1482,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -1514,10 +1511,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1543,10 +1540,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D4">
         <v>9</v>
@@ -1572,10 +1569,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1601,10 +1598,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1630,10 +1627,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -1659,10 +1656,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1688,10 +1685,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1717,10 +1714,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1746,10 +1743,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1788,163 +1785,163 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" t="s">
         <v>205</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>206</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>207</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>208</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>209</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>210</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>211</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>212</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>213</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>214</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>215</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>216</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>218</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>219</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>220</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>221</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>222</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>223</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>224</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>225</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>226</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>227</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>228</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>229</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>230</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>231</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>232</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>233</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>234</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>235</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>236</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>237</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>238</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>239</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>240</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>241</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>242</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>243</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>244</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>245</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>246</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>247</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>248</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>249</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>250</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>251</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>252</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>253</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>254</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:54">
@@ -1952,13 +1949,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
         <v>256</v>
-      </c>
-      <c r="C2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D2" t="s">
-        <v>257</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2113,13 +2110,13 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" t="s">
         <v>258</v>
-      </c>
-      <c r="C3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" t="s">
-        <v>259</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2274,13 +2271,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2435,13 +2432,13 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
         <v>261</v>
-      </c>
-      <c r="C5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" t="s">
-        <v>262</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -2596,13 +2593,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" t="s">
         <v>263</v>
-      </c>
-      <c r="C6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" t="s">
-        <v>264</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2757,13 +2754,13 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2918,13 +2915,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3079,13 +3076,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -3240,13 +3237,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -3401,13 +3398,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -3562,13 +3559,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3723,13 +3720,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -3884,13 +3881,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -4045,13 +4042,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -4206,13 +4203,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -4367,13 +4364,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>274</v>
+      </c>
+      <c r="C17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" t="s">
         <v>275</v>
-      </c>
-      <c r="C17" t="s">
-        <v>161</v>
-      </c>
-      <c r="D17" t="s">
-        <v>276</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -4528,13 +4525,13 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -4689,13 +4686,13 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -4850,13 +4847,13 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
+        <v>278</v>
+      </c>
+      <c r="C20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" t="s">
         <v>279</v>
-      </c>
-      <c r="C20" t="s">
-        <v>164</v>
-      </c>
-      <c r="D20" t="s">
-        <v>280</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -5011,13 +5008,13 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -5172,13 +5169,13 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -5346,55 +5343,55 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
         <v>283</v>
       </c>
-      <c r="C1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>284</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>285</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>286</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>287</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>288</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>289</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>290</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>291</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>292</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>293</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>294</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>295</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>296</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>297</v>
-      </c>
-      <c r="R1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -5402,10 +5399,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D2">
         <v>17052021</v>
@@ -5444,7 +5441,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q2">
         <v>400</v>
@@ -5455,10 +5452,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3">
         <v>17122021</v>
@@ -5497,7 +5494,7 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q3">
         <v>100</v>
@@ -5508,10 +5505,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4">
         <v>28032021</v>
@@ -5550,7 +5547,7 @@
         <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q4">
         <v>200</v>
@@ -5561,10 +5558,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5">
         <v>17052021</v>
@@ -5603,7 +5600,7 @@
         <v>2</v>
       </c>
       <c r="P5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q5">
         <v>100</v>
@@ -5614,10 +5611,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6">
         <v>3082021</v>
@@ -5656,7 +5653,7 @@
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q6">
         <v>400</v>
@@ -5667,10 +5664,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D7">
         <v>17112021</v>
@@ -5709,7 +5706,7 @@
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q7">
         <v>100</v>
@@ -5720,10 +5717,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8">
         <v>12082021</v>
@@ -5762,7 +5759,7 @@
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q8">
         <v>100</v>
@@ -5773,10 +5770,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D9">
         <v>11012022</v>
@@ -5815,7 +5812,7 @@
         <v>2</v>
       </c>
       <c r="P9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Q9">
         <v>300</v>
@@ -5826,10 +5823,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10">
         <v>28062021</v>
@@ -5868,7 +5865,7 @@
         <v>2</v>
       </c>
       <c r="P10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Q10">
         <v>200</v>
@@ -5879,10 +5876,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11">
         <v>17082021</v>
@@ -5921,7 +5918,7 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Q11">
         <v>200</v>
@@ -5945,16 +5942,16 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" t="s">
         <v>317</v>
       </c>
-      <c r="C1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>318</v>
-      </c>
-      <c r="E1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5962,13 +5959,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D2" t="s">
         <v>320</v>
-      </c>
-      <c r="C2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D2" t="s">
-        <v>321</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -5979,13 +5976,13 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>321</v>
+      </c>
+      <c r="C3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" t="s">
         <v>322</v>
-      </c>
-      <c r="C3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D3" t="s">
-        <v>323</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -5996,13 +5993,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" t="s">
         <v>324</v>
-      </c>
-      <c r="C4" t="s">
-        <v>303</v>
-      </c>
-      <c r="D4" t="s">
-        <v>325</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6013,13 +6010,13 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D5" t="s">
         <v>326</v>
-      </c>
-      <c r="C5" t="s">
-        <v>305</v>
-      </c>
-      <c r="D5" t="s">
-        <v>327</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6030,13 +6027,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D6" t="s">
         <v>328</v>
-      </c>
-      <c r="C6" t="s">
-        <v>307</v>
-      </c>
-      <c r="D6" t="s">
-        <v>329</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6047,13 +6044,13 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C7" t="s">
+        <v>308</v>
+      </c>
+      <c r="D7" t="s">
         <v>330</v>
-      </c>
-      <c r="C7" t="s">
-        <v>309</v>
-      </c>
-      <c r="D7" t="s">
-        <v>331</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6064,13 +6061,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8" t="s">
+        <v>310</v>
+      </c>
+      <c r="D8" t="s">
         <v>332</v>
-      </c>
-      <c r="C8" t="s">
-        <v>311</v>
-      </c>
-      <c r="D8" t="s">
-        <v>333</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -6081,13 +6078,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
+        <v>333</v>
+      </c>
+      <c r="C9" t="s">
+        <v>311</v>
+      </c>
+      <c r="D9" t="s">
         <v>334</v>
-      </c>
-      <c r="C9" t="s">
-        <v>312</v>
-      </c>
-      <c r="D9" t="s">
-        <v>335</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -6098,13 +6095,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>335</v>
+      </c>
+      <c r="C10" t="s">
+        <v>313</v>
+      </c>
+      <c r="D10" t="s">
         <v>336</v>
-      </c>
-      <c r="C10" t="s">
-        <v>314</v>
-      </c>
-      <c r="D10" t="s">
-        <v>337</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6115,13 +6112,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>337</v>
+      </c>
+      <c r="C11" t="s">
+        <v>315</v>
+      </c>
+      <c r="D11" t="s">
         <v>338</v>
-      </c>
-      <c r="C11" t="s">
-        <v>316</v>
-      </c>
-      <c r="D11" t="s">
-        <v>339</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -6132,13 +6129,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -6149,13 +6146,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -6179,28 +6176,28 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1" t="s">
         <v>342</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>343</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>344</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>345</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>346</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>347</v>
-      </c>
-      <c r="I1" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -6208,7 +6205,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -6234,7 +6231,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C3">
         <v>99</v>
@@ -6260,7 +6257,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -6286,7 +6283,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -6312,7 +6309,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -6338,7 +6335,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -6364,7 +6361,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -6390,7 +6387,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -6416,7 +6413,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C10">
         <v>11</v>
@@ -6442,7 +6439,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -6749,13 +6746,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -6798,16 +6795,13 @@
       <c r="N1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -6831,24 +6825,21 @@
         <v>27072021</v>
       </c>
       <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2">
         <v>9</v>
       </c>
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
       <c r="M2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -6872,24 +6863,21 @@
         <v>20062021</v>
       </c>
       <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
       </c>
       <c r="M3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>54</v>
-      </c>
-      <c r="N3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -6913,24 +6901,21 @@
         <v>30082021</v>
       </c>
       <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>55</v>
       </c>
       <c r="M4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>56</v>
-      </c>
-      <c r="N4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -6954,24 +6939,21 @@
         <v>30072021</v>
       </c>
       <c r="J5">
-        <v>3</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>57</v>
       </c>
       <c r="M5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>58</v>
-      </c>
-      <c r="N5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
@@ -6995,24 +6977,21 @@
         <v>1092021</v>
       </c>
       <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6">
         <v>9</v>
       </c>
+      <c r="L6" t="s">
+        <v>59</v>
+      </c>
       <c r="M6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>60</v>
-      </c>
-      <c r="N6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -7038,22 +7017,19 @@
       <c r="J7">
         <v>2</v>
       </c>
-      <c r="K7">
-        <v>2</v>
+      <c r="L7" t="s">
+        <v>61</v>
       </c>
       <c r="M7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>62</v>
-      </c>
-      <c r="N7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
@@ -7079,22 +7055,19 @@
       <c r="J8">
         <v>2</v>
       </c>
-      <c r="K8">
-        <v>2</v>
+      <c r="L8" t="s">
+        <v>63</v>
       </c>
       <c r="M8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>64</v>
-      </c>
-      <c r="N8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -7118,24 +7091,21 @@
         <v>21022021</v>
       </c>
       <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>65</v>
       </c>
       <c r="M9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>66</v>
-      </c>
-      <c r="N9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>67</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -7159,24 +7129,21 @@
         <v>12102021</v>
       </c>
       <c r="J10">
-        <v>2</v>
-      </c>
-      <c r="K10">
         <v>9</v>
       </c>
+      <c r="L10" t="s">
+        <v>67</v>
+      </c>
       <c r="M10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
         <v>68</v>
-      </c>
-      <c r="N10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
@@ -7200,15 +7167,12 @@
         <v>12052021</v>
       </c>
       <c r="J11">
-        <v>2</v>
-      </c>
-      <c r="K11">
         <v>9</v>
       </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
       <c r="M11" t="s">
-        <v>70</v>
-      </c>
-      <c r="N11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -7230,46 +7194,46 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
         <v>38</v>
       </c>
       <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>73</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>74</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>75</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>76</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>78</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>79</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>80</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>81</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>82</v>
-      </c>
-      <c r="O1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -7277,10 +7241,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -7310,7 +7274,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N2">
         <v>3</v>
@@ -7321,10 +7285,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -7354,7 +7318,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N3">
         <v>9</v>
@@ -7365,10 +7329,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -7409,40 +7373,40 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
-        <v>89</v>
       </c>
       <c r="N5">
         <v>3</v>
@@ -7453,10 +7417,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -7497,10 +7461,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -7530,7 +7494,7 @@
         <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N7">
         <v>3</v>
@@ -7541,10 +7505,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -7585,10 +7549,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -7629,10 +7593,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -7662,7 +7626,7 @@
         <v>4</v>
       </c>
       <c r="M10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N10">
         <v>4</v>
@@ -7673,10 +7637,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -7706,7 +7670,7 @@
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N11">
         <v>3</v>
@@ -7730,19 +7694,19 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
         <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" t="s">
         <v>40</v>
@@ -7751,58 +7715,58 @@
         <v>41</v>
       </c>
       <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
         <v>100</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>101</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>102</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>103</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>104</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>105</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>106</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>107</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>108</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" t="s">
         <v>109</v>
       </c>
-      <c r="S1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>110</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>111</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>112</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>113</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>114</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>115</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>116</v>
       </c>
       <c r="AA1" t="s">
         <v>42</v>
@@ -7811,10 +7775,10 @@
         <v>43</v>
       </c>
       <c r="AC1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD1" t="s">
         <v>117</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -7822,7 +7786,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -7903,7 +7867,7 @@
         <v>7</v>
       </c>
       <c r="AC2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:30">
@@ -7911,7 +7875,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -7992,10 +7956,10 @@
         <v>4</v>
       </c>
       <c r="AC3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD3" t="s">
         <v>122</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -8003,7 +7967,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
@@ -8084,7 +8048,7 @@
         <v>4</v>
       </c>
       <c r="AC4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -8092,7 +8056,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
@@ -8173,7 +8137,7 @@
         <v>6</v>
       </c>
       <c r="AC5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -8181,7 +8145,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
         <v>32</v>
@@ -8262,7 +8226,7 @@
         <v>8</v>
       </c>
       <c r="AC6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:30">
@@ -8270,7 +8234,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -8348,7 +8312,7 @@
         <v>8</v>
       </c>
       <c r="AC7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -8356,7 +8320,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
@@ -8437,7 +8401,7 @@
         <v>5</v>
       </c>
       <c r="AC8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -8445,7 +8409,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
         <v>36</v>
@@ -8526,7 +8490,7 @@
         <v>9</v>
       </c>
       <c r="AC9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -8534,7 +8498,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
         <v>36</v>
@@ -8615,7 +8579,7 @@
         <v>5</v>
       </c>
       <c r="AC10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -8623,7 +8587,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
@@ -8701,7 +8665,7 @@
         <v>8</v>
       </c>
       <c r="AC11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -8719,13 +8683,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
         <v>140</v>
-      </c>
-      <c r="B1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" t="s">
-        <v>141</v>
       </c>
       <c r="D1" t="s">
         <v>38</v>
@@ -8736,13 +8700,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8750,13 +8714,13 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8764,13 +8728,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8778,13 +8742,13 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -8792,13 +8756,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -8806,13 +8770,13 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -8820,13 +8784,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -8834,13 +8798,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -8848,13 +8812,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -8862,13 +8826,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -8889,19 +8853,19 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>143</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>144</v>
-      </c>
-      <c r="F1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -8909,10 +8873,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D2">
         <v>27012021</v>
@@ -8926,10 +8890,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D3">
         <v>6022021</v>
@@ -8943,10 +8907,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4">
         <v>26092020</v>
@@ -8960,10 +8924,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5">
         <v>19012021</v>
@@ -8977,10 +8941,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6">
         <v>17032021</v>
@@ -8994,10 +8958,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D7">
         <v>20102020</v>
@@ -9011,10 +8975,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D8">
         <v>4062021</v>
@@ -9028,10 +8992,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D9">
         <v>16082020</v>
@@ -9045,10 +9009,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D10">
         <v>1072021</v>
@@ -9062,10 +9026,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11">
         <v>26092020</v>
@@ -9079,10 +9043,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12">
         <v>6082020</v>
@@ -9096,10 +9060,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13">
         <v>21032021</v>
@@ -9113,10 +9077,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D14">
         <v>18012021</v>
@@ -9130,10 +9094,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D15">
         <v>21012021</v>
@@ -9147,10 +9111,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D16">
         <v>17082020</v>
@@ -9164,10 +9128,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D17">
         <v>15122020</v>
@@ -9181,10 +9145,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D18">
         <v>22102020</v>
@@ -9198,10 +9162,10 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19">
         <v>25102020</v>
@@ -9215,10 +9179,10 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D20">
         <v>26042021</v>
@@ -9232,10 +9196,10 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21">
         <v>19082020</v>
@@ -9249,10 +9213,10 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D22">
         <v>27072021</v>
@@ -9279,58 +9243,58 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" t="s">
         <v>167</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>168</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>169</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>170</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>171</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>172</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>173</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>174</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>175</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>176</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>177</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>178</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>179</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>180</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>181</v>
-      </c>
-      <c r="S1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -9338,10 +9302,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -9394,10 +9358,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -9450,10 +9414,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -9506,10 +9470,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -9562,10 +9526,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D6">
         <v>4</v>

</xml_diff>